<commit_message>
max iscrizioni per interfaccia di didattica
</commit_message>
<xml_diff>
--- a/template/Template Studenti Import 1.0.xlsx
+++ b/template/Template Studenti Import 1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Studenti" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t># Template per Import Studenti</t>
   </si>
@@ -28,8 +28,8 @@
         <color rgb="FFCC0000"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve">N.B.: Effettuare una copia del file e lavorare sulla copia.
-Version: 1.0
+      <t xml:space="preserve"># N.B.: Effettuare una copia del file e lavorare sulla copia.
+# Version: 1.0
 </t>
     </r>
     <r>
@@ -55,12 +55,15 @@
   <si>
     <t>Classe</t>
   </si>
+  <si>
+    <t>Anno</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -76,6 +79,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <b/>
       <sz val="11.0"/>
@@ -103,12 +107,28 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -123,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -133,22 +153,17 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -380,23 +395,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -1397,6 +1414,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>